<commit_message>
Refactoring the monolithic code to smaller functions.
</commit_message>
<xml_diff>
--- a/performance-anaysis.xlsx
+++ b/performance-anaysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,6 +127,186 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>110455.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>220940.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>331522.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>445665.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>559424.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>671659.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>784015.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>895047.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.006737E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.11746E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.228457E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$1:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.494600306428E12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.494600308003E12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.494600312176E12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.494600318923E12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.494600328253E12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.494600340698E12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.494600355394E12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.494600372872E12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4946003934E12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.494600416524E12</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.494600442585E12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.494600471586E12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2140780168"/>
+        <c:axId val="-2140782488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2140780168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2140782488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2140782488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2140780168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
@@ -726,8 +906,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2113314840"/>
-        <c:axId val="-2114957672"/>
+        <c:axId val="2147027656"/>
+        <c:axId val="2147034968"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1319,11 +1499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062195224"/>
-        <c:axId val="-2106847160"/>
+        <c:axId val="2147047096"/>
+        <c:axId val="2147040888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2113314840"/>
+        <c:axId val="2147027656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,12 +1532,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114957672"/>
+        <c:crossAx val="2147034968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2114957672"/>
+        <c:axId val="2147034968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,12 +1583,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2113314840"/>
+        <c:crossAx val="2147027656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2106847160"/>
+        <c:axId val="2147040888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1453,12 +1633,12 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2062195224"/>
+        <c:crossAx val="2147047096"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2062195224"/>
+        <c:axId val="2147047096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1468,7 +1648,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2106847160"/>
+        <c:crossAx val="2147040888"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -1499,6 +1680,41 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1857,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" activeCellId="1" sqref="E1:E12 G1:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2148,6 +2364,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2160,7 +2377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>